<commit_message>
update download xls files and get sample info sql cmd
</commit_message>
<xml_diff>
--- a/ONMATHLIMS/lims_app/static/download/downmachine.xlsx
+++ b/ONMATHLIMS/lims_app/static/download/downmachine.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -144,12 +144,12 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>